<commit_message>
Section_4 WIP, finished upto video# 23
</commit_message>
<xml_diff>
--- a/Time_Series_Analysis_Forecasting_ML_Git.xlsx
+++ b/Time_Series_Analysis_Forecasting_ML_Git.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\unpat\_Projects\Time_Series_Analysis_Forecasting_ML\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1605EB43-2188-48D8-9D9D-E7E69706C431}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5520548-F8DD-4093-B870-D1C8D418637A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -553,7 +553,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="J14" sqref="J14"/>
+      <selection pane="bottomRight" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -612,11 +612,11 @@
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
       <c r="E4" s="12">
-        <f t="shared" ref="E4:E12" si="0">D4-C4</f>
+        <f t="shared" ref="E4:E8" si="0">D4-C4</f>
         <v>0</v>
       </c>
       <c r="F4" s="13">
-        <f>SUM(E4:E10)</f>
+        <f>SUM(E4:E6)</f>
         <v>0</v>
       </c>
       <c r="G4" s="14" t="s">
@@ -658,11 +658,23 @@
       <c r="A7" s="15">
         <v>4</v>
       </c>
-      <c r="B7" s="16"/>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="19"/>
+      <c r="B7" s="16">
+        <v>44758</v>
+      </c>
+      <c r="C7" s="17">
+        <v>0.90625</v>
+      </c>
+      <c r="D7" s="17">
+        <v>0.96875</v>
+      </c>
+      <c r="E7" s="12">
+        <f t="shared" si="0"/>
+        <v>6.25E-2</v>
+      </c>
+      <c r="F7" s="13">
+        <f>SUM(E7:E10)</f>
+        <v>6.25E-2</v>
+      </c>
       <c r="G7" s="19"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
@@ -670,7 +682,10 @@
       <c r="B8" s="16"/>
       <c r="C8" s="17"/>
       <c r="D8" s="17"/>
-      <c r="E8" s="18"/>
+      <c r="E8" s="18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="F8" s="19"/>
       <c r="G8" s="19"/>
     </row>

</xml_diff>

<commit_message>
Section_4 WIP, finished upto video# 25
</commit_message>
<xml_diff>
--- a/Time_Series_Analysis_Forecasting_ML_Git.xlsx
+++ b/Time_Series_Analysis_Forecasting_ML_Git.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\unpat\_Projects\Time_Series_Analysis_Forecasting_ML\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5520548-F8DD-4093-B870-D1C8D418637A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B41B15BA-DE28-4748-98A3-8F692CD7C9CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -183,7 +183,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -258,6 +258,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -553,7 +556,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="D7" sqref="D7"/>
+      <selection pane="bottomRight" activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -655,16 +658,16 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="15">
+      <c r="A7" s="9">
         <v>4</v>
       </c>
-      <c r="B7" s="16">
-        <v>44758</v>
-      </c>
-      <c r="C7" s="17">
+      <c r="B7" s="10">
+        <v>44820</v>
+      </c>
+      <c r="C7" s="11">
         <v>0.90625</v>
       </c>
-      <c r="D7" s="17">
+      <c r="D7" s="11">
         <v>0.96875</v>
       </c>
       <c r="E7" s="12">
@@ -672,48 +675,72 @@
         <v>6.25E-2</v>
       </c>
       <c r="F7" s="13">
-        <f>SUM(E7:E10)</f>
-        <v>6.25E-2</v>
+        <f>SUM(E7:E16)</f>
+        <v>0.22916666666666674</v>
       </c>
       <c r="G7" s="19"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="15"/>
-      <c r="B8" s="16"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
+      <c r="B8" s="16">
+        <v>44822</v>
+      </c>
+      <c r="C8" s="17">
+        <v>0.44791666666666669</v>
+      </c>
+      <c r="D8" s="17">
+        <v>0.53125</v>
+      </c>
       <c r="E8" s="18">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>8.3333333333333315E-2</v>
       </c>
       <c r="F8" s="19"/>
       <c r="G8" s="19"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="15"/>
-      <c r="B9" s="16"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="18"/>
+      <c r="B9" s="16">
+        <v>44823</v>
+      </c>
+      <c r="C9" s="17">
+        <v>0.94791666666666663</v>
+      </c>
+      <c r="D9" s="17">
+        <v>0.98958333333333337</v>
+      </c>
+      <c r="E9" s="18">
+        <f t="shared" ref="E9" si="1">D9-C9</f>
+        <v>4.1666666666666741E-2</v>
+      </c>
       <c r="F9" s="19"/>
       <c r="G9" s="19"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="21"/>
-      <c r="B10" s="22"/>
-      <c r="C10" s="23"/>
-      <c r="D10" s="23"/>
-      <c r="E10" s="24"/>
-      <c r="F10" s="25"/>
+      <c r="A10" s="15"/>
+      <c r="B10" s="16">
+        <v>44824</v>
+      </c>
+      <c r="C10" s="17">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="D10" s="17">
+        <v>5.2083333333333336E-2</v>
+      </c>
+      <c r="E10" s="18">
+        <f t="shared" ref="E10" si="2">D10-C10</f>
+        <v>4.1666666666666671E-2</v>
+      </c>
+      <c r="F10" s="19"/>
       <c r="G10" s="19"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="9"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="13"/>
+      <c r="A11" s="15"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="26"/>
       <c r="G11" s="19"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
@@ -756,21 +783,21 @@
       <c r="G15" s="19"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="21"/>
-      <c r="B16" s="22"/>
-      <c r="C16" s="23"/>
-      <c r="D16" s="23"/>
-      <c r="E16" s="24"/>
-      <c r="F16" s="25"/>
+      <c r="A16" s="15"/>
+      <c r="B16" s="16"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="19"/>
       <c r="G16" s="19"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" s="9"/>
-      <c r="B17" s="10"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="13"/>
+      <c r="A17" s="15"/>
+      <c r="B17" s="16"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="26"/>
       <c r="G17" s="19"/>
       <c r="H17" s="1" t="s">
         <v>5</v>
@@ -843,21 +870,21 @@
       <c r="G24" s="19"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A25" s="21"/>
-      <c r="B25" s="22"/>
-      <c r="C25" s="23"/>
-      <c r="D25" s="23"/>
-      <c r="E25" s="24"/>
-      <c r="F25" s="25"/>
+      <c r="A25" s="15"/>
+      <c r="B25" s="16"/>
+      <c r="C25" s="17"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="19"/>
       <c r="G25" s="19"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A26" s="9"/>
-      <c r="B26" s="10"/>
-      <c r="C26" s="11"/>
-      <c r="D26" s="11"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="13"/>
+      <c r="A26" s="15"/>
+      <c r="B26" s="16"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="17"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="26"/>
       <c r="G26" s="19"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
@@ -891,21 +918,21 @@
       <c r="G29" s="19"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A30" s="21"/>
-      <c r="B30" s="22"/>
-      <c r="C30" s="23"/>
-      <c r="D30" s="23"/>
-      <c r="E30" s="24"/>
-      <c r="F30" s="25"/>
+      <c r="A30" s="15"/>
+      <c r="B30" s="16"/>
+      <c r="C30" s="17"/>
+      <c r="D30" s="17"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="19"/>
       <c r="G30" s="19"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A31" s="9"/>
-      <c r="B31" s="10"/>
-      <c r="C31" s="11"/>
-      <c r="D31" s="11"/>
-      <c r="E31" s="12"/>
-      <c r="F31" s="13"/>
+      <c r="A31" s="15"/>
+      <c r="B31" s="16"/>
+      <c r="C31" s="17"/>
+      <c r="D31" s="17"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="26"/>
       <c r="G31" s="19"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Section_4 WIP, finished upto lesson# 27
</commit_message>
<xml_diff>
--- a/Time_Series_Analysis_Forecasting_ML_Git.xlsx
+++ b/Time_Series_Analysis_Forecasting_ML_Git.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\unpat\_Projects\Time_Series_Analysis_Forecasting_ML\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B41B15BA-DE28-4748-98A3-8F692CD7C9CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C0249C0-DA6D-4D5C-92EC-9EE815CFFF0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="13">
   <si>
     <t>Date</t>
   </si>
@@ -71,13 +71,16 @@
   </si>
   <si>
     <t>1, 2, 3</t>
+  </si>
+  <si>
+    <t>Finished upto lesson 27</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -109,6 +112,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -183,7 +192,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -261,6 +270,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="20" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -556,7 +568,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="I13" sqref="I13"/>
+      <selection pane="bottomRight" activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -675,8 +687,8 @@
         <v>6.25E-2</v>
       </c>
       <c r="F7" s="13">
-        <f>SUM(E7:E16)</f>
-        <v>0.22916666666666674</v>
+        <f>SUM(E7:E23)</f>
+        <v>0.34375000000000006</v>
       </c>
       <c r="G7" s="19"/>
     </row>
@@ -736,21 +748,41 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="15"/>
-      <c r="B11" s="16"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="26"/>
+      <c r="B11" s="16">
+        <v>44824</v>
+      </c>
+      <c r="C11" s="17">
+        <v>0.48958333333333331</v>
+      </c>
+      <c r="D11" s="17">
+        <v>0.53125</v>
+      </c>
+      <c r="E11" s="18">
+        <f t="shared" ref="E11" si="3">D11-C11</f>
+        <v>4.1666666666666685E-2</v>
+      </c>
+      <c r="F11" s="19"/>
       <c r="G11" s="19"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="15"/>
-      <c r="B12" s="16"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="18"/>
+      <c r="B12" s="16">
+        <v>44824</v>
+      </c>
+      <c r="C12" s="17">
+        <v>0.5625</v>
+      </c>
+      <c r="D12" s="17">
+        <v>0.63541666666666663</v>
+      </c>
+      <c r="E12" s="18">
+        <f t="shared" ref="E12" si="4">D12-C12</f>
+        <v>7.291666666666663E-2</v>
+      </c>
       <c r="F12" s="19"/>
-      <c r="G12" s="20"/>
+      <c r="G12" s="27" t="s">
+        <v>12</v>
+      </c>
       <c r="H12" s="1" t="s">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
Section_4 WIP, finished upto lesson# 29 - Holt's Linear Trend model
</commit_message>
<xml_diff>
--- a/Time_Series_Analysis_Forecasting_ML_Git.xlsx
+++ b/Time_Series_Analysis_Forecasting_ML_Git.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\unpat\_Projects\Time_Series_Analysis_Forecasting_ML\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C0249C0-DA6D-4D5C-92EC-9EE815CFFF0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA14BC3F-AEB3-4EB7-9322-5FAE4A610D45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -73,7 +73,10 @@
     <t>1, 2, 3</t>
   </si>
   <si>
-    <t>Finished upto lesson 27</t>
+    <t>Finished upto lesson# 27</t>
+  </si>
+  <si>
+    <t>Finished upto lesson# 29</t>
   </si>
 </sst>
 </file>
@@ -568,7 +571,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="G13" sqref="G13"/>
+      <selection pane="bottomRight" activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -688,7 +691,7 @@
       </c>
       <c r="F7" s="13">
         <f>SUM(E7:E23)</f>
-        <v>0.34375000000000006</v>
+        <v>0.39583333333333343</v>
       </c>
       <c r="G7" s="19"/>
     </row>
@@ -789,12 +792,23 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="15"/>
-      <c r="B13" s="16"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="18"/>
+      <c r="B13" s="16">
+        <v>44825</v>
+      </c>
+      <c r="C13" s="17">
+        <v>0.90625</v>
+      </c>
+      <c r="D13" s="17">
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="E13" s="18">
+        <f t="shared" ref="E13" si="5">D13-C13</f>
+        <v>5.208333333333337E-2</v>
+      </c>
       <c r="F13" s="19"/>
-      <c r="G13" s="19"/>
+      <c r="G13" s="27" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="15"/>

</xml_diff>

<commit_message>
Section_4 WIP, finished upto lesson# 31 - Holt-Winters
</commit_message>
<xml_diff>
--- a/Time_Series_Analysis_Forecasting_ML_Git.xlsx
+++ b/Time_Series_Analysis_Forecasting_ML_Git.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\unpat\_Projects\Time_Series_Analysis_Forecasting_ML\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA14BC3F-AEB3-4EB7-9322-5FAE4A610D45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0733133-5045-41F9-8B67-16FC8FDA20E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="15">
   <si>
     <t>Date</t>
   </si>
@@ -77,6 +77,9 @@
   </si>
   <si>
     <t>Finished upto lesson# 29</t>
+  </si>
+  <si>
+    <t>Finished upto lesson# 31</t>
   </si>
 </sst>
 </file>
@@ -568,7 +571,7 @@
   <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
       <selection pane="bottomRight" activeCell="G14" sqref="G14"/>
@@ -691,7 +694,7 @@
       </c>
       <c r="F7" s="13">
         <f>SUM(E7:E23)</f>
-        <v>0.39583333333333343</v>
+        <v>0.4479166666666668</v>
       </c>
       <c r="G7" s="19"/>
     </row>
@@ -812,12 +815,23 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="15"/>
-      <c r="B14" s="16"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="18"/>
+      <c r="B14" s="16">
+        <v>44826</v>
+      </c>
+      <c r="C14" s="17">
+        <v>0.9375</v>
+      </c>
+      <c r="D14" s="17">
+        <v>0.98958333333333337</v>
+      </c>
+      <c r="E14" s="18">
+        <f t="shared" ref="E14" si="6">D14-C14</f>
+        <v>5.208333333333337E-2</v>
+      </c>
       <c r="F14" s="19"/>
-      <c r="G14" s="19"/>
+      <c r="G14" s="27" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="15"/>

</xml_diff>

<commit_message>
Finished Section_4 (upto lesson# 39)
</commit_message>
<xml_diff>
--- a/Time_Series_Analysis_Forecasting_ML_Git.xlsx
+++ b/Time_Series_Analysis_Forecasting_ML_Git.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\unpat\_Projects\Time_Series_Analysis_Forecasting_ML\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0733133-5045-41F9-8B67-16FC8FDA20E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B51578BB-4263-4579-939D-9448D4064B77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="16">
   <si>
     <t>Date</t>
   </si>
@@ -80,6 +80,9 @@
   </si>
   <si>
     <t>Finished upto lesson# 31</t>
+  </si>
+  <si>
+    <t>Finished section 4 (upto lesson# 39)</t>
   </si>
 </sst>
 </file>
@@ -198,7 +201,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -279,6 +282,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -571,10 +577,10 @@
   <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="G14" sqref="G14"/>
+      <selection pane="bottomRight" activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -665,12 +671,12 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="21"/>
-      <c r="B6" s="22"/>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="25"/>
+      <c r="A6" s="15"/>
+      <c r="B6" s="16"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="19"/>
       <c r="G6" s="19" t="s">
         <v>7</v>
       </c>
@@ -694,9 +700,9 @@
       </c>
       <c r="F7" s="13">
         <f>SUM(E7:E23)</f>
-        <v>0.4479166666666668</v>
-      </c>
-      <c r="G7" s="19"/>
+        <v>0.66666666666666685</v>
+      </c>
+      <c r="G7" s="14"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="15"/>
@@ -835,24 +841,46 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="15"/>
-      <c r="B15" s="16"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="18"/>
+      <c r="B15" s="16">
+        <v>44827</v>
+      </c>
+      <c r="C15" s="17">
+        <v>0.40625</v>
+      </c>
+      <c r="D15" s="17">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="E15" s="18">
+        <f t="shared" ref="E15" si="7">D15-C15</f>
+        <v>0.13541666666666663</v>
+      </c>
       <c r="F15" s="19"/>
       <c r="G15" s="19"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="15"/>
-      <c r="B16" s="16"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="19"/>
-      <c r="G16" s="19"/>
+      <c r="A16" s="21"/>
+      <c r="B16" s="22">
+        <v>44827</v>
+      </c>
+      <c r="C16" s="23">
+        <v>0.59375</v>
+      </c>
+      <c r="D16" s="23">
+        <v>0.67708333333333337</v>
+      </c>
+      <c r="E16" s="24">
+        <f t="shared" ref="E16" si="8">D16-C16</f>
+        <v>8.333333333333337E-2</v>
+      </c>
+      <c r="F16" s="25"/>
+      <c r="G16" s="28" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" s="15"/>
+      <c r="A17" s="15">
+        <v>5</v>
+      </c>
       <c r="B17" s="16"/>
       <c r="C17" s="17"/>
       <c r="D17" s="17"/>

</xml_diff>

<commit_message>
Section_5 WIP, finished upto video# 43
</commit_message>
<xml_diff>
--- a/Time_Series_Analysis_Forecasting_ML_Git.xlsx
+++ b/Time_Series_Analysis_Forecasting_ML_Git.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\unpat\_Projects\Time_Series_Analysis_Forecasting_ML\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B51578BB-4263-4579-939D-9448D4064B77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D486480A-DA3E-4411-BD75-4B58A3F3CA78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
   <si>
     <t>Date</t>
   </si>
@@ -83,6 +83,9 @@
   </si>
   <si>
     <t>Finished section 4 (upto lesson# 39)</t>
+  </si>
+  <si>
+    <t>Section 5, finished upto lesson# 43</t>
   </si>
 </sst>
 </file>
@@ -577,10 +580,10 @@
   <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="L9" sqref="L9"/>
+      <selection pane="bottomRight" activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -700,7 +703,7 @@
       </c>
       <c r="F7" s="13">
         <f>SUM(E7:E23)</f>
-        <v>0.66666666666666685</v>
+        <v>0.75000000000000022</v>
       </c>
       <c r="G7" s="14"/>
     </row>
@@ -869,7 +872,7 @@
         <v>0.67708333333333337</v>
       </c>
       <c r="E16" s="24">
-        <f t="shared" ref="E16" si="8">D16-C16</f>
+        <f t="shared" ref="E16:E17" si="8">D16-C16</f>
         <v>8.333333333333337E-2</v>
       </c>
       <c r="F16" s="25"/>
@@ -881,12 +884,26 @@
       <c r="A17" s="15">
         <v>5</v>
       </c>
-      <c r="B17" s="16"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="26"/>
-      <c r="G17" s="19"/>
+      <c r="B17" s="10">
+        <v>44828</v>
+      </c>
+      <c r="C17" s="11">
+        <v>0.85416666666666663</v>
+      </c>
+      <c r="D17" s="11">
+        <v>0.9375</v>
+      </c>
+      <c r="E17" s="12">
+        <f t="shared" si="8"/>
+        <v>8.333333333333337E-2</v>
+      </c>
+      <c r="F17" s="13">
+        <f>SUM(E17:E33)</f>
+        <v>8.333333333333337E-2</v>
+      </c>
+      <c r="G17" s="19" t="s">
+        <v>16</v>
+      </c>
       <c r="H17" s="1" t="s">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
Section_5 WIP, finished upto video# 44
</commit_message>
<xml_diff>
--- a/Time_Series_Analysis_Forecasting_ML_Git.xlsx
+++ b/Time_Series_Analysis_Forecasting_ML_Git.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\unpat\_Projects\Time_Series_Analysis_Forecasting_ML\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D486480A-DA3E-4411-BD75-4B58A3F3CA78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{558E1BEC-CE60-4C1D-A8F9-6512D8834F87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="18">
   <si>
     <t>Date</t>
   </si>
@@ -86,6 +86,9 @@
   </si>
   <si>
     <t>Section 5, finished upto lesson# 43</t>
+  </si>
+  <si>
+    <t>Section 5, finished upto lesson# 44</t>
   </si>
 </sst>
 </file>
@@ -580,10 +583,10 @@
   <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="G17" sqref="G17"/>
+      <selection pane="bottomRight" activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -703,7 +706,7 @@
       </c>
       <c r="F7" s="13">
         <f>SUM(E7:E23)</f>
-        <v>0.75000000000000022</v>
+        <v>0.83333333333333348</v>
       </c>
       <c r="G7" s="14"/>
     </row>
@@ -872,7 +875,7 @@
         <v>0.67708333333333337</v>
       </c>
       <c r="E16" s="24">
-        <f t="shared" ref="E16:E17" si="8">D16-C16</f>
+        <f t="shared" ref="E16:E18" si="8">D16-C16</f>
         <v>8.333333333333337E-2</v>
       </c>
       <c r="F16" s="25"/>
@@ -881,7 +884,7 @@
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" s="15">
+      <c r="A17" s="9">
         <v>5</v>
       </c>
       <c r="B17" s="10">
@@ -899,9 +902,9 @@
       </c>
       <c r="F17" s="13">
         <f>SUM(E17:E33)</f>
-        <v>8.333333333333337E-2</v>
-      </c>
-      <c r="G17" s="19" t="s">
+        <v>0.16666666666666663</v>
+      </c>
+      <c r="G17" s="14" t="s">
         <v>16</v>
       </c>
       <c r="H17" s="1" t="s">
@@ -910,12 +913,23 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="15"/>
-      <c r="B18" s="16"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="18"/>
+      <c r="B18" s="16">
+        <v>44830</v>
+      </c>
+      <c r="C18" s="17">
+        <v>0.89583333333333337</v>
+      </c>
+      <c r="D18" s="17">
+        <v>0.97916666666666663</v>
+      </c>
+      <c r="E18" s="18">
+        <f t="shared" si="8"/>
+        <v>8.3333333333333259E-2</v>
+      </c>
       <c r="F18" s="19"/>
-      <c r="G18" s="20"/>
+      <c r="G18" s="27" t="s">
+        <v>17</v>
+      </c>
       <c r="H18" s="1" t="s">
         <v>5</v>
       </c>
@@ -1053,13 +1067,13 @@
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A33" s="15"/>
-      <c r="B33" s="16"/>
-      <c r="C33" s="17"/>
-      <c r="D33" s="17"/>
-      <c r="E33" s="18"/>
-      <c r="F33" s="19"/>
-      <c r="G33" s="19"/>
+      <c r="A33" s="21"/>
+      <c r="B33" s="22"/>
+      <c r="C33" s="23"/>
+      <c r="D33" s="23"/>
+      <c r="E33" s="24"/>
+      <c r="F33" s="25"/>
+      <c r="G33" s="25"/>
       <c r="H33" s="1" t="s">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
Section_5 WIP, finished upto video# 45
</commit_message>
<xml_diff>
--- a/Time_Series_Analysis_Forecasting_ML_Git.xlsx
+++ b/Time_Series_Analysis_Forecasting_ML_Git.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\unpat\_Projects\Time_Series_Analysis_Forecasting_ML\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{558E1BEC-CE60-4C1D-A8F9-6512D8834F87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1FA2847-D7AC-4DA9-9CF3-84FDC26226B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
   <si>
     <t>Date</t>
   </si>
@@ -89,6 +89,9 @@
   </si>
   <si>
     <t>Section 5, finished upto lesson# 44</t>
+  </si>
+  <si>
+    <t>Section 5, finished upto lesson# 45</t>
   </si>
 </sst>
 </file>
@@ -586,7 +589,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="G18" sqref="G18"/>
+      <selection pane="bottomRight" activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -706,7 +709,7 @@
       </c>
       <c r="F7" s="13">
         <f>SUM(E7:E23)</f>
-        <v>0.83333333333333348</v>
+        <v>0.91666666666666685</v>
       </c>
       <c r="G7" s="14"/>
     </row>
@@ -902,7 +905,7 @@
       </c>
       <c r="F17" s="13">
         <f>SUM(E17:E33)</f>
-        <v>0.16666666666666663</v>
+        <v>0.25</v>
       </c>
       <c r="G17" s="14" t="s">
         <v>16</v>
@@ -936,12 +939,23 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="15"/>
-      <c r="B19" s="16"/>
-      <c r="C19" s="17"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="18"/>
+      <c r="B19" s="16">
+        <v>44832</v>
+      </c>
+      <c r="C19" s="17">
+        <v>0.84375</v>
+      </c>
+      <c r="D19" s="17">
+        <v>0.92708333333333337</v>
+      </c>
+      <c r="E19" s="18">
+        <f t="shared" ref="E19" si="9">D19-C19</f>
+        <v>8.333333333333337E-2</v>
+      </c>
       <c r="F19" s="19"/>
-      <c r="G19" s="19"/>
+      <c r="G19" s="27" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="15"/>

</xml_diff>

<commit_message>
Section_5 WIP, finished upto video# 46
</commit_message>
<xml_diff>
--- a/Time_Series_Analysis_Forecasting_ML_Git.xlsx
+++ b/Time_Series_Analysis_Forecasting_ML_Git.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\unpat\_Projects\Time_Series_Analysis_Forecasting_ML\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1FA2847-D7AC-4DA9-9CF3-84FDC26226B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03509A6D-6CBB-43FD-9084-022C4A21D695}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -98,7 +98,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -132,6 +132,15 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -210,7 +219,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -294,6 +303,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="18" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -959,10 +971,19 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="15"/>
-      <c r="B20" s="16"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="18"/>
+      <c r="B20" s="16">
+        <v>44835</v>
+      </c>
+      <c r="C20" s="17">
+        <v>0.90625</v>
+      </c>
+      <c r="D20" s="29">
+        <v>0.90625</v>
+      </c>
+      <c r="E20" s="18">
+        <f t="shared" ref="E20" si="10">D20-C20</f>
+        <v>0</v>
+      </c>
       <c r="F20" s="19"/>
       <c r="G20" s="19"/>
     </row>

</xml_diff>

<commit_message>
Section_5 WIP, finished upto lesson# 48
</commit_message>
<xml_diff>
--- a/Time_Series_Analysis_Forecasting_ML_Git.xlsx
+++ b/Time_Series_Analysis_Forecasting_ML_Git.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\unpat\_Projects\Time_Series_Analysis_Forecasting_ML\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03509A6D-6CBB-43FD-9084-022C4A21D695}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0F426CE-C5EE-4700-B0C3-73C5610E69A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
   <si>
     <t>Date</t>
   </si>
@@ -92,13 +92,19 @@
   </si>
   <si>
     <t>Section 5, finished upto lesson# 45</t>
+  </si>
+  <si>
+    <t>Section 5, finished upto lesson# 46</t>
+  </si>
+  <si>
+    <t>Section 5, finished upto lesson# 48</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -132,15 +138,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <i/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -219,7 +216,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -303,9 +300,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="18" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -601,7 +595,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="G20" sqref="G20"/>
+      <selection pane="bottomRight" activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -721,7 +715,7 @@
       </c>
       <c r="F7" s="13">
         <f>SUM(E7:E23)</f>
-        <v>0.91666666666666685</v>
+        <v>1.041666666666667</v>
       </c>
       <c r="G7" s="14"/>
     </row>
@@ -917,7 +911,7 @@
       </c>
       <c r="F17" s="13">
         <f>SUM(E17:E33)</f>
-        <v>0.25</v>
+        <v>0.37500000000000011</v>
       </c>
       <c r="G17" s="14" t="s">
         <v>16</v>
@@ -977,24 +971,37 @@
       <c r="C20" s="17">
         <v>0.90625</v>
       </c>
-      <c r="D20" s="29">
-        <v>0.90625</v>
+      <c r="D20" s="17">
+        <v>0.98958333333333337</v>
       </c>
       <c r="E20" s="18">
         <f t="shared" ref="E20" si="10">D20-C20</f>
-        <v>0</v>
+        <v>8.333333333333337E-2</v>
       </c>
       <c r="F20" s="19"/>
-      <c r="G20" s="19"/>
+      <c r="G20" s="27" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="15"/>
-      <c r="B21" s="16"/>
-      <c r="C21" s="17"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="18"/>
+      <c r="B21" s="16">
+        <v>44836</v>
+      </c>
+      <c r="C21" s="17">
+        <v>0.85416666666666663</v>
+      </c>
+      <c r="D21" s="17">
+        <v>0.89583333333333337</v>
+      </c>
+      <c r="E21" s="18">
+        <f t="shared" ref="E21" si="11">D21-C21</f>
+        <v>4.1666666666666741E-2</v>
+      </c>
       <c r="F21" s="19"/>
-      <c r="G21" s="19"/>
+      <c r="G21" s="27" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="15"/>

</xml_diff>